<commit_message>
After Meeting. Much to do
</commit_message>
<xml_diff>
--- a/Dokumente/VergleichRandomWalk.xlsx
+++ b/Dokumente/VergleichRandomWalk.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="10">
   <si>
     <t>Normal 20% Random</t>
   </si>
@@ -33,12 +33,27 @@
   <si>
     <t>Mit Index</t>
   </si>
+  <si>
+    <t>Stats</t>
+  </si>
+  <si>
+    <t>Anzahl Knoten</t>
+  </si>
+  <si>
+    <t>Anzahl Relationen</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,6 +65,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,11 +97,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1379,25 +1402,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="94521984"/>
-        <c:axId val="95609216"/>
+        <c:axId val="90262144"/>
+        <c:axId val="91152768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94521984"/>
+        <c:axId val="90262144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95609216"/>
+        <c:crossAx val="91152768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95609216"/>
+        <c:axId val="91152768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1405,7 +1428,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94521984"/>
+        <c:crossAx val="90262144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1417,7 +1440,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1518,25 +1541,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="95646080"/>
-        <c:axId val="95647616"/>
+        <c:axId val="91189632"/>
+        <c:axId val="91191168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95646080"/>
+        <c:axId val="91189632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95647616"/>
+        <c:crossAx val="91191168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95647616"/>
+        <c:axId val="91191168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1544,7 +1567,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95646080"/>
+        <c:crossAx val="91189632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1556,7 +1579,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000029" r="0.70000000000000029" t="0.78740157499999996" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3570,10 +3593,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -3887,6 +3910,35 @@
         <v>28.073098425651779</v>
       </c>
     </row>
+    <row r="19" spans="6:7">
+      <c r="F19" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7">
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7">
+      <c r="F21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="4">
+        <v>2286</v>
+      </c>
+    </row>
+    <row r="22" spans="6:7">
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3894,10 +3946,367 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D9"/>
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="2">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3">
+        <v>1000</v>
+      </c>
+      <c r="B3">
+        <v>425473</v>
+      </c>
+      <c r="C3">
+        <v>562458</v>
+      </c>
+      <c r="D3">
+        <f>100-100/B3*C3</f>
+        <v>-32.195932526858343</v>
+      </c>
+      <c r="G3">
+        <v>1000</v>
+      </c>
+      <c r="H3">
+        <v>369569</v>
+      </c>
+      <c r="I3">
+        <v>420317</v>
+      </c>
+      <c r="J3">
+        <f>100-100/H3*I3</f>
+        <v>-13.731671217012249</v>
+      </c>
+      <c r="M3">
+        <v>1000</v>
+      </c>
+      <c r="N3">
+        <v>282086</v>
+      </c>
+      <c r="O3">
+        <v>309547</v>
+      </c>
+      <c r="P3">
+        <f>100-100/N3*O3</f>
+        <v>-9.7349744404188812</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4">
+        <v>2000</v>
+      </c>
+      <c r="B4">
+        <v>810756</v>
+      </c>
+      <c r="C4">
+        <v>990162</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D9" si="0">100-100/B4*C4</f>
+        <v>-22.128235868744738</v>
+      </c>
+      <c r="G4">
+        <v>2000</v>
+      </c>
+      <c r="H4">
+        <v>698738</v>
+      </c>
+      <c r="I4">
+        <v>851941</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J9" si="1">100-100/H4*I4</f>
+        <v>-21.925671710998969</v>
+      </c>
+      <c r="M4">
+        <v>2000</v>
+      </c>
+      <c r="N4">
+        <v>482858</v>
+      </c>
+      <c r="O4">
+        <v>540868</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P9" si="2">100-100/N4*O4</f>
+        <v>-12.013883999022482</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5">
+        <v>4000</v>
+      </c>
+      <c r="B5">
+        <v>1610042</v>
+      </c>
+      <c r="C5">
+        <v>2025982</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>-25.834108675425867</v>
+      </c>
+      <c r="G5">
+        <v>4000</v>
+      </c>
+      <c r="H5">
+        <v>1404513</v>
+      </c>
+      <c r="I5">
+        <v>1655459</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>-17.867118353479114</v>
+      </c>
+      <c r="M5">
+        <v>4000</v>
+      </c>
+      <c r="N5">
+        <v>1013149</v>
+      </c>
+      <c r="O5">
+        <v>1193947</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="2"/>
+        <v>-17.845154069144812</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6">
+        <v>8000</v>
+      </c>
+      <c r="B6">
+        <v>3659360</v>
+      </c>
+      <c r="C6">
+        <v>4254039</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>-16.250901797035539</v>
+      </c>
+      <c r="G6">
+        <v>8000</v>
+      </c>
+      <c r="H6">
+        <v>3238254</v>
+      </c>
+      <c r="I6">
+        <v>3690378</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>-13.961968394079037</v>
+      </c>
+      <c r="M6">
+        <v>8000</v>
+      </c>
+      <c r="N6">
+        <v>2435938</v>
+      </c>
+      <c r="O6">
+        <v>2544448</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="2"/>
+        <v>-4.4545468727036592</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7">
+        <v>16000</v>
+      </c>
+      <c r="B7">
+        <v>8912382</v>
+      </c>
+      <c r="C7">
+        <v>9449676</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-6.0286239974902429</v>
+      </c>
+      <c r="G7">
+        <v>16000</v>
+      </c>
+      <c r="H7">
+        <v>7815457</v>
+      </c>
+      <c r="I7">
+        <v>7661092</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>1.9751244233062693</v>
+      </c>
+      <c r="M7">
+        <v>16000</v>
+      </c>
+      <c r="N7">
+        <v>6305451</v>
+      </c>
+      <c r="O7">
+        <v>6172980</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="2"/>
+        <v>2.1008965100196662</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8">
+        <v>32000</v>
+      </c>
+      <c r="B8">
+        <v>23325922</v>
+      </c>
+      <c r="C8">
+        <v>22979091</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1.4868908504452776</v>
+      </c>
+      <c r="G8">
+        <v>32000</v>
+      </c>
+      <c r="H8">
+        <v>20120361</v>
+      </c>
+      <c r="I8">
+        <v>19712096</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>2.0291136923437847</v>
+      </c>
+      <c r="M8">
+        <v>32000</v>
+      </c>
+      <c r="N8">
+        <v>17294057</v>
+      </c>
+      <c r="O8">
+        <v>16650959</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="2"/>
+        <v>3.7186069179718828</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9">
+        <v>64000</v>
+      </c>
+      <c r="B9">
+        <v>69918922</v>
+      </c>
+      <c r="C9">
+        <v>63648713</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>8.9678284799642682</v>
+      </c>
+      <c r="G9">
+        <v>64000</v>
+      </c>
+      <c r="H9">
+        <v>64472764</v>
+      </c>
+      <c r="I9">
+        <v>60549805</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>6.0846763138617774</v>
+      </c>
+      <c r="M9">
+        <v>64000</v>
+      </c>
+      <c r="N9">
+        <v>58693443</v>
+      </c>
+      <c r="O9">
+        <v>50728744</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="2"/>
+        <v>13.569997929751707</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="E16" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6">
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17">
+        <v>63044</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6">
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>106653</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6">
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19">
+        <v>70.099999999999994</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -3906,6 +4315,9 @@
       <c r="A1" s="2">
         <v>1</v>
       </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="G1" s="2">
         <v>0.2</v>
       </c>
@@ -3929,40 +4341,40 @@
         <v>1000</v>
       </c>
       <c r="B3">
-        <v>425473</v>
+        <v>934175</v>
       </c>
       <c r="C3">
-        <v>562458</v>
+        <v>1282831</v>
       </c>
       <c r="D3">
         <f>100-100/B3*C3</f>
-        <v>-32.195932526858343</v>
+        <v>-37.322343244038848</v>
       </c>
       <c r="G3">
         <v>1000</v>
       </c>
       <c r="H3">
-        <v>369569</v>
+        <v>13281080</v>
       </c>
       <c r="I3">
-        <v>420317</v>
+        <v>4178424</v>
       </c>
       <c r="J3">
         <f>100-100/H3*I3</f>
-        <v>-13.731671217012249</v>
+        <v>68.538522469558202</v>
       </c>
       <c r="M3">
         <v>1000</v>
       </c>
       <c r="N3">
-        <v>282086</v>
+        <v>870768</v>
       </c>
       <c r="O3">
-        <v>309547</v>
+        <v>1162917</v>
       </c>
       <c r="P3">
         <f>100-100/N3*O3</f>
-        <v>-9.7349744404188812</v>
+        <v>-33.550727633537292</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -3970,333 +4382,6 @@
         <v>2000</v>
       </c>
       <c r="B4">
-        <v>810756</v>
-      </c>
-      <c r="C4">
-        <v>990162</v>
-      </c>
-      <c r="D4">
-        <f t="shared" ref="D4:D9" si="0">100-100/B4*C4</f>
-        <v>-22.128235868744738</v>
-      </c>
-      <c r="G4">
-        <v>2000</v>
-      </c>
-      <c r="H4">
-        <v>698738</v>
-      </c>
-      <c r="I4">
-        <v>851941</v>
-      </c>
-      <c r="J4">
-        <f t="shared" ref="J4:J9" si="1">100-100/H4*I4</f>
-        <v>-21.925671710998969</v>
-      </c>
-      <c r="M4">
-        <v>2000</v>
-      </c>
-      <c r="N4">
-        <v>482858</v>
-      </c>
-      <c r="O4">
-        <v>540868</v>
-      </c>
-      <c r="P4">
-        <f t="shared" ref="P4:P9" si="2">100-100/N4*O4</f>
-        <v>-12.013883999022482</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5">
-        <v>4000</v>
-      </c>
-      <c r="B5">
-        <v>1610042</v>
-      </c>
-      <c r="C5">
-        <v>2025982</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>-25.834108675425867</v>
-      </c>
-      <c r="G5">
-        <v>4000</v>
-      </c>
-      <c r="H5">
-        <v>1404513</v>
-      </c>
-      <c r="I5">
-        <v>1655459</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="1"/>
-        <v>-17.867118353479114</v>
-      </c>
-      <c r="M5">
-        <v>4000</v>
-      </c>
-      <c r="N5">
-        <v>1013149</v>
-      </c>
-      <c r="O5">
-        <v>1193947</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="2"/>
-        <v>-17.845154069144812</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6">
-        <v>8000</v>
-      </c>
-      <c r="B6">
-        <v>3659360</v>
-      </c>
-      <c r="C6">
-        <v>4254039</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>-16.250901797035539</v>
-      </c>
-      <c r="G6">
-        <v>8000</v>
-      </c>
-      <c r="H6">
-        <v>3238254</v>
-      </c>
-      <c r="I6">
-        <v>3690378</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="1"/>
-        <v>-13.961968394079037</v>
-      </c>
-      <c r="M6">
-        <v>8000</v>
-      </c>
-      <c r="N6">
-        <v>2435938</v>
-      </c>
-      <c r="O6">
-        <v>2544448</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="2"/>
-        <v>-4.4545468727036592</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7">
-        <v>16000</v>
-      </c>
-      <c r="B7">
-        <v>8912382</v>
-      </c>
-      <c r="C7">
-        <v>9449676</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>-6.0286239974902429</v>
-      </c>
-      <c r="G7">
-        <v>16000</v>
-      </c>
-      <c r="H7">
-        <v>7815457</v>
-      </c>
-      <c r="I7">
-        <v>7661092</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="1"/>
-        <v>1.9751244233062693</v>
-      </c>
-      <c r="M7">
-        <v>16000</v>
-      </c>
-      <c r="N7">
-        <v>6305451</v>
-      </c>
-      <c r="O7">
-        <v>6172980</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="2"/>
-        <v>2.1008965100196662</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8">
-        <v>32000</v>
-      </c>
-      <c r="B8">
-        <v>23325922</v>
-      </c>
-      <c r="C8">
-        <v>22979091</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>1.4868908504452776</v>
-      </c>
-      <c r="G8">
-        <v>32000</v>
-      </c>
-      <c r="H8">
-        <v>20120361</v>
-      </c>
-      <c r="I8">
-        <v>19712096</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="1"/>
-        <v>2.0291136923437847</v>
-      </c>
-      <c r="M8">
-        <v>32000</v>
-      </c>
-      <c r="N8">
-        <v>17294057</v>
-      </c>
-      <c r="O8">
-        <v>16650959</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="2"/>
-        <v>3.7186069179718828</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9">
-        <v>64000</v>
-      </c>
-      <c r="B9">
-        <v>69918922</v>
-      </c>
-      <c r="C9">
-        <v>63648713</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>8.9678284799642682</v>
-      </c>
-      <c r="G9">
-        <v>64000</v>
-      </c>
-      <c r="H9">
-        <v>64472764</v>
-      </c>
-      <c r="I9">
-        <v>60549805</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="1"/>
-        <v>6.0846763138617774</v>
-      </c>
-      <c r="M9">
-        <v>64000</v>
-      </c>
-      <c r="N9">
-        <v>58693443</v>
-      </c>
-      <c r="O9">
-        <v>50728744</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="2"/>
-        <v>13.569997929751707</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P41"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="2">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="M1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3">
-        <v>1000</v>
-      </c>
-      <c r="B3">
-        <v>934175</v>
-      </c>
-      <c r="C3">
-        <v>1282831</v>
-      </c>
-      <c r="D3">
-        <f>100-100/B3*C3</f>
-        <v>-37.322343244038848</v>
-      </c>
-      <c r="G3">
-        <v>1000</v>
-      </c>
-      <c r="H3">
-        <v>13281080</v>
-      </c>
-      <c r="I3">
-        <v>4178424</v>
-      </c>
-      <c r="J3">
-        <f>100-100/H3*I3</f>
-        <v>68.538522469558202</v>
-      </c>
-      <c r="M3">
-        <v>1000</v>
-      </c>
-      <c r="N3">
-        <v>870768</v>
-      </c>
-      <c r="O3">
-        <v>1162917</v>
-      </c>
-      <c r="P3">
-        <f>100-100/N3*O3</f>
-        <v>-33.550727633537292</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4">
-        <v>2000</v>
-      </c>
-      <c r="B4">
         <v>1743722</v>
       </c>
       <c r="C4">
@@ -4305,6 +4390,9 @@
       <c r="D4">
         <f t="shared" ref="D4:D9" si="0">100-100/B4*C4</f>
         <v>-31.938405319196534</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
       </c>
       <c r="G4">
         <v>2000</v>
@@ -4909,6 +4997,9 @@
         <f t="shared" si="6"/>
         <v>-20.313728304265638</v>
       </c>
+      <c r="J29" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="1:16">
       <c r="A30">
@@ -4924,6 +5015,12 @@
         <f t="shared" si="6"/>
         <v>-17.073787029435721</v>
       </c>
+      <c r="J30" t="s">
+        <v>6</v>
+      </c>
+      <c r="K30" s="4">
+        <v>103002</v>
+      </c>
     </row>
     <row r="31" spans="1:16">
       <c r="A31">
@@ -4939,6 +5036,12 @@
         <f t="shared" si="6"/>
         <v>-14.428149471971267</v>
       </c>
+      <c r="J31" t="s">
+        <v>7</v>
+      </c>
+      <c r="K31">
+        <v>1999821</v>
+      </c>
     </row>
     <row r="32" spans="1:16">
       <c r="A32">
@@ -4953,6 +5056,12 @@
       <c r="D32">
         <f t="shared" si="6"/>
         <v>-13.051189734811388</v>
+      </c>
+      <c r="J32" t="s">
+        <v>8</v>
+      </c>
+      <c r="K32">
+        <v>239.09</v>
       </c>
     </row>
     <row r="33" spans="1:4">

</xml_diff>